<commit_message>
Excel: Compte converti en texte (sans .0)
</commit_message>
<xml_diff>
--- a/factures_comptables_brutes.xlsx
+++ b/factures_comptables_brutes.xlsx
@@ -1,20 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arles/Projets/analyse_comptable/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D27BE433-C759-3D42-A27F-6A8DC986D81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="16940" yWindow="3320" windowWidth="31760" windowHeight="21740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -68,16 +86,19 @@
   </si>
   <si>
     <t>Erreur</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,25 +150,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -185,7 +215,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -219,6 +249,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -253,9 +284,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -428,14 +460,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="2" max="2" width="32" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,11 +489,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>45390</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C2" t="s">
@@ -463,22 +503,22 @@
         <v>1526.33</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>45380</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D3">
         <v>377.38</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>45394</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
@@ -488,11 +528,11 @@
         <v>-534.41</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>45404</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
@@ -502,11 +542,11 @@
         <v>1337.65</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>45393</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" t="s">
@@ -516,11 +556,11 @@
         <v>717</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
@@ -530,11 +570,11 @@
         <v>2409.33</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>45416</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
@@ -544,33 +584,33 @@
         <v>2656.34</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>45303</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D9">
         <v>2267.6</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>45415</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D10">
         <v>2699.79</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>45409</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
@@ -580,11 +620,11 @@
         <v>1711.97</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>45397</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
@@ -594,22 +634,22 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>45397</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D13">
         <v>953.52</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>45298</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C14" t="s">
@@ -619,22 +659,22 @@
         <v>1666.95</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>45421</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D15">
         <v>-7.65</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>45381</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
@@ -644,22 +684,22 @@
         <v>-830.03</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>45464</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D17">
-        <v>2611.07</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>2611.0700000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>45413</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
@@ -669,44 +709,49 @@
         <v>453.9</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>45388</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D19">
         <v>229.55</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>45365</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D20">
         <v>11.44</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>45466</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="D21">
         <v>724.66</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>45470</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
@@ -716,11 +761,11 @@
         <v>2495.11</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>45422</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
@@ -730,11 +775,11 @@
         <v>968.62</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>45442</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C25" t="s">
@@ -744,36 +789,36 @@
         <v>1253.78</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>45471</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C26" t="s">
         <v>15</v>
       </c>
       <c r="D26">
-        <v>-97.45999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>-97.46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>45344</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D27">
-        <v>2230.03</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>2230.0300000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>45435</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C28" t="s">
@@ -783,11 +828,11 @@
         <v>-829.04</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>45390</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C29" t="s">
@@ -797,25 +842,25 @@
         <v>-388.15</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>45462</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C30" t="s">
         <v>13</v>
       </c>
       <c r="D30">
-        <v>560.1900000000001</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>560.19000000000005</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>45316</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C31" t="s">
@@ -825,22 +870,22 @@
         <v>2029.85</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>45440</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D32">
-        <v>1121.16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>1121.1600000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>45448</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C33" t="s">
@@ -850,11 +895,11 @@
         <v>1032.33</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>45320</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C34" t="s">
@@ -864,11 +909,11 @@
         <v>1505.18</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>45332</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C35" t="s">
@@ -878,11 +923,11 @@
         <v>-867.39</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>45443</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C36" t="s">
@@ -892,33 +937,33 @@
         <v>-935.87</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>45303</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D37">
         <v>-353.82</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>45430</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D38">
-        <v>-522.3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>-522.29999999999995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>45369</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C39" t="s">
@@ -928,11 +973,11 @@
         <v>-450.33</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>45351</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C40" t="s">
@@ -942,11 +987,11 @@
         <v>-189.95</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>45416</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C41" t="s">
@@ -956,11 +1001,11 @@
         <v>2963.48</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>45407</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C42" t="s">
@@ -970,33 +1015,33 @@
         <v>-363.86</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>45342</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D43">
         <v>-58.43</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>45389</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D44">
         <v>-559.98</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>45441</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C45" t="s">
@@ -1006,11 +1051,11 @@
         <v>1781.6</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>45398</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C46" t="s">
@@ -1020,11 +1065,11 @@
         <v>2604.73</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>45322</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C47" t="s">
@@ -1034,11 +1079,11 @@
         <v>455.21</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>45408</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C48" t="s">
@@ -1048,22 +1093,22 @@
         <v>1895.69</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>45292</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D49">
         <v>1085.26</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>45293</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C50" t="s">
@@ -1073,11 +1118,11 @@
         <v>-437.55</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>45388</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C51" t="s">

</xml_diff>